<commit_message>
PDS 12 May - Pandas Stacking, Concat, Merging Operations
</commit_message>
<xml_diff>
--- a/output/pandas/dataset.xlsx
+++ b/output/pandas/dataset.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,6 +484,11 @@
           <t>Start Date</t>
         </is>
       </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Umrank</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -531,6 +536,9 @@
           <t>Mar 1943</t>
         </is>
       </c>
+      <c r="L2" t="n">
+        <v>7.5</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -578,6 +586,9 @@
           <t>Jan 1920</t>
         </is>
       </c>
+      <c r="L3" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -625,6 +636,9 @@
           <t>Feb 1960</t>
         </is>
       </c>
+      <c r="L4" t="n">
+        <v>7.5</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -672,6 +686,9 @@
           <t>Apr 1950</t>
         </is>
       </c>
+      <c r="L5" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -719,6 +736,9 @@
           <t>Aug 1928</t>
         </is>
       </c>
+      <c r="L6" t="n">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -766,6 +786,9 @@
           <t>Mar 1920</t>
         </is>
       </c>
+      <c r="L7" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -813,6 +836,9 @@
           <t>Oct 1971</t>
         </is>
       </c>
+      <c r="L8" t="n">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -860,6 +886,9 @@
           <t>Apr 1925</t>
         </is>
       </c>
+      <c r="L9" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -907,6 +936,9 @@
           <t>Nov 1930</t>
         </is>
       </c>
+      <c r="L10" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -954,6 +986,9 @@
           <t>Jan 1994</t>
         </is>
       </c>
+      <c r="L11" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -1000,6 +1035,9 @@
         <is>
           <t>Jun 1974</t>
         </is>
+      </c>
+      <c r="L12" t="n">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>